<commit_message>
2. Scrapped more webpages 'product_description, 'home_page_url' , 'product_link'
</commit_message>
<xml_diff>
--- a/output/https___mrawholesale_com.xlsx
+++ b/output/https___mrawholesale_com.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bob Marley</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bluntlife</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -517,7 +517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Special Blue Pocket Torch,3"Dual Mini Plastic (20PC CT) )</t>
+          <t xml:space="preserve">Special Blue Pocket Torch,3"Dual Mini Plastic (20PC CT) </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://mrawholesale.com/products/SPECIAL-BLUE-POCKET-TORCH-2-5-CLASSIC-RUBBER-LIGTER-20CT-p572907865</t>
+          <t>https://mrawholesale.com/products/SPECIAL-BLUE-POCKET-TORCH-2-5-CLASSIC-RUBBER-LIGHTER-20CT-p572907865</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SOUL</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -644,6 +644,276 @@
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MAGNETIC TRAY WITH COVER SMALL</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/MAGNETIC-TRAY-WITH-COVER-SMALL-p572926723</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MAGENTIC TRAY WITH 3D DESIGN WITH COVER SMALL</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/MAGENTIC-TRAY-WITH-3D-DESIGN-WITH-COVER-SMALL-p572927701</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MAGNETIC TRAY MDEIUM SIZE ASSORTED</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/MAGNETIC-TRAY-MDEIUM-SIZE-ASSORTED-p572927736</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MAGNETIC TRAY 3D DESIGN MIDIUM SIZE</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/MAGNETIC-TRAY-3D-DESIGN-MIDIUM-SIZE-p572927739</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BLUNTLIFE 24CT LARGE INCENSE STICK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/BLUNTLIFE-24CT-LARGE-INCENSE-STICK-p572929820</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BLUNTLIFE 72CT SMALL INCENSE STICK</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/BLUNTLIFE-72CT-SMALL-INCENSE-STICK-p572927961</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BLUNTLIFE 20CT SPRAY</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/BLUNTLIFE-20CT-SPRAY-p572932779</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BEE ONE HEATER 10138</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/BEE-ONE-HEATER-10138-p598951019</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5.5" HEAVY PIPE 10139</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/5-5-HEAVY-PIPE-10139-p598951037</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>5" HEAVY PIPE WITH SMALL HANDLE 10140</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://mrawholesale.com/products/5-HEAVY-PIPE-WITH-SMALL-HANDLE-10140-p598950090</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['n/a']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>https://mrawholesale.com/</t>
         </is>

</xml_diff>